<commit_message>
Updated docs a bit further. Added a PDF of the pin map
</commit_message>
<xml_diff>
--- a/Docs/CPU Pin Map.xlsx
+++ b/Docs/CPU Pin Map.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="379" uniqueCount="244">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="251">
   <si>
     <t>PE2</t>
   </si>
@@ -633,9 +633,6 @@
     <t>Crystal</t>
   </si>
   <si>
-    <t>To driver</t>
-  </si>
-  <si>
     <t>Cooling Fan Enable</t>
   </si>
   <si>
@@ -660,15 +657,6 @@
     <t>I2C-SDA - FM24CL64B F-RAM</t>
   </si>
   <si>
-    <t>SPI1-SCK W25Q128JV</t>
-  </si>
-  <si>
-    <t>SPI1-MISO W25Q128JV</t>
-  </si>
-  <si>
-    <t>SPI1-MOSI W25Q128JV</t>
-  </si>
-  <si>
     <t>CS W25Q128JV</t>
   </si>
   <si>
@@ -748,6 +736,39 @@
   </si>
   <si>
     <t>USB</t>
+  </si>
+  <si>
+    <t>LCD Con - Encoder button</t>
+  </si>
+  <si>
+    <t>LCD Con - Encoder B</t>
+  </si>
+  <si>
+    <t>LCD Con - Encoder A</t>
+  </si>
+  <si>
+    <t>LCD Con - backlight maybe</t>
+  </si>
+  <si>
+    <t>LCD Con - LCD something</t>
+  </si>
+  <si>
+    <t>SPI1-SCK W25Q128JV/Touch</t>
+  </si>
+  <si>
+    <t>SPI1-MISO W25Q128JV/Touch</t>
+  </si>
+  <si>
+    <t>SPI1-MOSI W25Q128JV/Touch</t>
+  </si>
+  <si>
+    <t>LCD Con - Touch EN?</t>
+  </si>
+  <si>
+    <t>LCD Con - touch something - int?</t>
+  </si>
+  <si>
+    <t>LCD Con - Buzzer Enable</t>
   </si>
 </sst>
 </file>
@@ -1123,8 +1144,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:M130"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B98" sqref="B98"/>
+    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
+      <selection activeCell="N90" sqref="N90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1143,7 +1164,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="C1">
         <v>3.3</v>
@@ -1157,7 +1178,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
       <c r="C2">
         <v>3.3</v>
@@ -1171,7 +1192,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="C3">
         <v>3.3</v>
@@ -1185,7 +1206,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="C4">
         <v>0</v>
@@ -1199,7 +1220,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="C5">
         <v>0</v>
@@ -1221,7 +1242,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="C7">
         <v>0</v>
@@ -1235,7 +1256,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="C8">
         <v>0.1</v>
@@ -1249,7 +1270,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C9">
         <v>0</v>
@@ -1309,7 +1330,7 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="C15">
         <v>3.3</v>
@@ -1323,7 +1344,7 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="C16">
         <v>3.3</v>
@@ -1332,12 +1353,12 @@
         <v>202</v>
       </c>
     </row>
-    <row r="17" spans="1:7">
+    <row r="17" spans="1:5">
       <c r="A17" s="3" t="s">
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="C17">
         <v>0</v>
@@ -1346,12 +1367,12 @@
         <v>201</v>
       </c>
     </row>
-    <row r="18" spans="1:7">
+    <row r="18" spans="1:5">
       <c r="A18" s="3" t="s">
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="C18">
         <v>0</v>
@@ -1360,7 +1381,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="19" spans="1:7">
+    <row r="19" spans="1:5">
       <c r="A19" t="s">
         <v>10</v>
       </c>
@@ -1368,7 +1389,7 @@
         <v>3.3</v>
       </c>
     </row>
-    <row r="20" spans="1:7">
+    <row r="20" spans="1:5">
       <c r="A20" t="s">
         <v>18</v>
       </c>
@@ -1376,7 +1397,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:7">
+    <row r="21" spans="1:5">
       <c r="A21" t="s">
         <v>19</v>
       </c>
@@ -1384,7 +1405,7 @@
         <v>3.3</v>
       </c>
     </row>
-    <row r="22" spans="1:7">
+    <row r="22" spans="1:5">
       <c r="A22" t="s">
         <v>20</v>
       </c>
@@ -1392,12 +1413,12 @@
         <v>3.3</v>
       </c>
     </row>
-    <row r="23" spans="1:7">
+    <row r="23" spans="1:5">
       <c r="A23" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C23">
         <v>0</v>
@@ -1408,16 +1429,13 @@
       <c r="E23" t="s">
         <v>152</v>
       </c>
-      <c r="G23" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7">
+    </row>
+    <row r="24" spans="1:5">
       <c r="A24" s="1" t="s">
         <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C24">
         <v>0</v>
@@ -1429,12 +1447,12 @@
         <v>153</v>
       </c>
     </row>
-    <row r="25" spans="1:7">
+    <row r="25" spans="1:5">
       <c r="A25" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B25" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C25">
         <v>0</v>
@@ -1446,12 +1464,12 @@
         <v>154</v>
       </c>
     </row>
-    <row r="26" spans="1:7">
+    <row r="26" spans="1:5">
       <c r="A26" s="1" t="s">
         <v>24</v>
       </c>
       <c r="B26" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="C26">
         <v>0</v>
@@ -1460,7 +1478,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="27" spans="1:7">
+    <row r="27" spans="1:5">
       <c r="A27" t="s">
         <v>9</v>
       </c>
@@ -1468,7 +1486,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:7">
+    <row r="28" spans="1:5">
       <c r="A28" t="s">
         <v>10</v>
       </c>
@@ -1476,12 +1494,12 @@
         <v>3.3</v>
       </c>
     </row>
-    <row r="29" spans="1:7">
+    <row r="29" spans="1:5">
       <c r="A29" s="1" t="s">
         <v>25</v>
       </c>
       <c r="B29" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="C29">
         <v>0</v>
@@ -1490,12 +1508,12 @@
         <v>200</v>
       </c>
     </row>
-    <row r="30" spans="1:7">
+    <row r="30" spans="1:5">
       <c r="A30" s="1" t="s">
         <v>26</v>
       </c>
       <c r="B30" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="C30">
         <v>3.3</v>
@@ -1504,12 +1522,12 @@
         <v>200</v>
       </c>
     </row>
-    <row r="31" spans="1:7">
+    <row r="31" spans="1:5">
       <c r="A31" s="1" t="s">
         <v>27</v>
       </c>
       <c r="B31" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="C31">
         <v>0</v>
@@ -1518,12 +1536,12 @@
         <v>200</v>
       </c>
     </row>
-    <row r="32" spans="1:7">
+    <row r="32" spans="1:5">
       <c r="A32" s="1" t="s">
         <v>28</v>
       </c>
       <c r="B32" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="C32">
         <v>0</v>
@@ -1537,7 +1555,7 @@
         <v>29</v>
       </c>
       <c r="B33" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="C33">
         <v>3.3</v>
@@ -1551,7 +1569,7 @@
         <v>30</v>
       </c>
       <c r="B34" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="C34">
         <v>0</v>
@@ -1565,7 +1583,7 @@
         <v>31</v>
       </c>
       <c r="B35" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="C35">
         <v>0</v>
@@ -1579,7 +1597,7 @@
         <v>32</v>
       </c>
       <c r="B36" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="C36">
         <v>3.3</v>
@@ -1593,7 +1611,7 @@
         <v>33</v>
       </c>
       <c r="B37" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="C37">
         <v>0</v>
@@ -1607,7 +1625,7 @@
         <v>34</v>
       </c>
       <c r="B38" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="C38">
         <v>0.1</v>
@@ -1624,7 +1642,7 @@
         <v>35</v>
       </c>
       <c r="B39" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="C39">
         <v>0.1</v>
@@ -1641,7 +1659,7 @@
         <v>36</v>
       </c>
       <c r="B40" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="C40">
         <v>0.1</v>
@@ -1658,7 +1676,7 @@
         <v>37</v>
       </c>
       <c r="B41" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="C41">
         <v>0.1</v>
@@ -1675,7 +1693,7 @@
         <v>38</v>
       </c>
       <c r="B42" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="C42">
         <v>0.1</v>
@@ -1692,7 +1710,7 @@
         <v>39</v>
       </c>
       <c r="B43" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="C43">
         <v>0.2</v>
@@ -1709,7 +1727,7 @@
         <v>40</v>
       </c>
       <c r="B44" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="C44">
         <v>0.1</v>
@@ -1726,7 +1744,7 @@
         <v>41</v>
       </c>
       <c r="B45" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="C45">
         <v>0.1</v>
@@ -1743,7 +1761,7 @@
         <v>42</v>
       </c>
       <c r="B46" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="C46">
         <v>0.1</v>
@@ -1760,7 +1778,7 @@
         <v>43</v>
       </c>
       <c r="B47" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="C47">
         <v>0</v>
@@ -1774,7 +1792,7 @@
         <v>44</v>
       </c>
       <c r="B48" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="C48">
         <v>3.3</v>
@@ -1804,7 +1822,7 @@
         <v>46</v>
       </c>
       <c r="B51" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="C51">
         <v>0.02</v>
@@ -1818,7 +1836,7 @@
         <v>47</v>
       </c>
       <c r="B52" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="C52">
         <v>0</v>
@@ -1832,7 +1850,7 @@
         <v>48</v>
       </c>
       <c r="B53" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="C53">
         <v>0</v>
@@ -1846,7 +1864,7 @@
         <v>49</v>
       </c>
       <c r="B54" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="C54">
         <v>0</v>
@@ -1860,7 +1878,7 @@
         <v>50</v>
       </c>
       <c r="B55" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="C55">
         <v>1</v>
@@ -1877,7 +1895,7 @@
         <v>51</v>
       </c>
       <c r="B56" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="C56">
         <v>1</v>
@@ -1894,7 +1912,7 @@
         <v>52</v>
       </c>
       <c r="B57" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="C57">
         <v>1</v>
@@ -1911,7 +1929,7 @@
         <v>53</v>
       </c>
       <c r="B58" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="C58">
         <v>3.3</v>
@@ -1928,7 +1946,7 @@
         <v>54</v>
       </c>
       <c r="B59" t="s">
-        <v>239</v>
+        <v>250</v>
       </c>
       <c r="C59">
         <v>0</v>
@@ -1942,7 +1960,7 @@
         <v>55</v>
       </c>
       <c r="B60" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="C60">
         <v>0.25</v>
@@ -1959,7 +1977,7 @@
         <v>56</v>
       </c>
       <c r="B61" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="C61">
         <v>0</v>
@@ -1976,7 +1994,7 @@
         <v>57</v>
       </c>
       <c r="B62" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="C62">
         <v>0</v>
@@ -1993,7 +2011,7 @@
         <v>58</v>
       </c>
       <c r="B63" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C63">
         <v>1.6</v>
@@ -2010,7 +2028,7 @@
         <v>59</v>
       </c>
       <c r="B64" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C64">
         <v>3.3</v>
@@ -2027,7 +2045,7 @@
         <v>60</v>
       </c>
       <c r="B65" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="C65">
         <v>3.3</v>
@@ -2041,7 +2059,7 @@
         <v>61</v>
       </c>
       <c r="B66" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="C66">
         <v>3.3</v>
@@ -2055,7 +2073,7 @@
         <v>62</v>
       </c>
       <c r="B67" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="C67">
         <v>3.3</v>
@@ -2069,7 +2087,7 @@
         <v>63</v>
       </c>
       <c r="B68" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="C68">
         <v>3.3</v>
@@ -2086,7 +2104,7 @@
         <v>64</v>
       </c>
       <c r="B69" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="C69">
         <v>3.3</v>
@@ -2103,7 +2121,7 @@
         <v>65</v>
       </c>
       <c r="B70" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="C70">
         <v>0</v>
@@ -2120,7 +2138,7 @@
         <v>66</v>
       </c>
       <c r="B71" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="C71">
         <v>0</v>
@@ -2195,7 +2213,7 @@
         <v>70</v>
       </c>
       <c r="B77" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="C77">
         <v>0</v>
@@ -2209,7 +2227,7 @@
         <v>71</v>
       </c>
       <c r="B78" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="C78">
         <v>3.3</v>
@@ -2223,7 +2241,7 @@
         <v>72</v>
       </c>
       <c r="B79" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="C79">
         <v>3.3</v>
@@ -2237,7 +2255,7 @@
         <v>73</v>
       </c>
       <c r="B80" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="C80">
         <v>0</v>
@@ -2251,7 +2269,7 @@
         <v>74</v>
       </c>
       <c r="B81" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="C81">
         <v>0</v>
@@ -2268,7 +2286,7 @@
         <v>75</v>
       </c>
       <c r="B82" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="C82">
         <v>0</v>
@@ -2285,7 +2303,7 @@
         <v>76</v>
       </c>
       <c r="B83" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="C83">
         <v>3.3</v>
@@ -2299,7 +2317,7 @@
         <v>77</v>
       </c>
       <c r="B84" t="s">
-        <v>239</v>
+        <v>243</v>
       </c>
       <c r="C84">
         <v>3.3</v>
@@ -2313,7 +2331,7 @@
         <v>78</v>
       </c>
       <c r="B85" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="C85">
         <v>3.3</v>
@@ -2330,7 +2348,7 @@
         <v>79</v>
       </c>
       <c r="B86" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="C86">
         <v>3.3</v>
@@ -2347,7 +2365,7 @@
         <v>80</v>
       </c>
       <c r="B87" t="s">
-        <v>239</v>
+        <v>244</v>
       </c>
       <c r="C87">
         <v>3.3</v>
@@ -2361,7 +2379,7 @@
         <v>81</v>
       </c>
       <c r="B88" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="C88">
         <v>3.3</v>
@@ -2378,7 +2396,7 @@
         <v>82</v>
       </c>
       <c r="B89" t="s">
-        <v>214</v>
+        <v>245</v>
       </c>
       <c r="C89">
         <v>0</v>
@@ -2395,7 +2413,7 @@
         <v>83</v>
       </c>
       <c r="B90" t="s">
-        <v>215</v>
+        <v>246</v>
       </c>
       <c r="C90">
         <v>3.3</v>
@@ -2412,7 +2430,7 @@
         <v>84</v>
       </c>
       <c r="B91" t="s">
-        <v>216</v>
+        <v>247</v>
       </c>
       <c r="C91">
         <v>3.3</v>
@@ -2429,7 +2447,7 @@
         <v>85</v>
       </c>
       <c r="B92" t="s">
-        <v>239</v>
+        <v>248</v>
       </c>
       <c r="C92">
         <v>3.3</v>
@@ -2443,7 +2461,7 @@
         <v>86</v>
       </c>
       <c r="B93" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="C93">
         <v>3.3</v>
@@ -2465,7 +2483,7 @@
         <v>88</v>
       </c>
       <c r="B95" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C95">
         <v>3.3</v>
@@ -2479,7 +2497,7 @@
         <v>89</v>
       </c>
       <c r="B96" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C96">
         <v>3.3</v>
@@ -2493,7 +2511,7 @@
         <v>90</v>
       </c>
       <c r="B97" t="s">
-        <v>239</v>
+        <v>249</v>
       </c>
       <c r="C97">
         <v>3.3</v>
@@ -2507,7 +2525,7 @@
         <v>91</v>
       </c>
       <c r="B98" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="C98">
         <v>0</v>
@@ -2825,6 +2843,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>